<commit_message>
Mise à jour journal de travail + documentation iso 27001
</commit_message>
<xml_diff>
--- a/Rendu/Journaux.xlsx
+++ b/Rendu/Journaux.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>Lancement du projet de Pré-TPI, téléchargement documents &amp; personnalisation, création des journaux, création Github</t>
+  </si>
+  <si>
+    <t>Recherche documentation</t>
+  </si>
+  <si>
+    <t>Normes ISO:27001 afin de créer un politique de sécurité de l'information pour mon entreprise</t>
   </si>
 </sst>
 </file>
@@ -461,7 +467,7 @@
   <dimension ref="A1:H270"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -528,68 +534,461 @@
         <v>0.10763888888888884</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="17" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="18" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="19" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="20" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="21" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="22" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="23" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="24" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="25" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="26" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="27" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="28" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="29" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="30" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="31" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="32" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="33" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="34" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="35" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="36" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="37" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="38" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="39" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="40" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="41" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="42" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="43" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="44" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="45" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="46" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="47" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="48" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="49" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="50" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="51" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="52" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="53" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="54" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="55" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="56" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="57" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="58" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="59" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="60" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="61" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="62" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="63" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="64" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>44958</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="H3" s="7">
+        <f t="shared" ref="H3:H50" si="0">G3-F3</f>
+        <v>6.597222222222221E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="8"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="8"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="H51" s="7">
+        <f>SUM(H2:H50)</f>
+        <v>0.17361111111111105</v>
+      </c>
+    </row>
+    <row r="52" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
     <row r="65" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
     <row r="66" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
     <row r="67" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Mise à jour documentation générale+Cahier des charges + organisations des dossiers
</commit_message>
<xml_diff>
--- a/Rendu/Journaux.xlsx
+++ b/Rendu/Journaux.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -107,6 +107,33 @@
   </si>
   <si>
     <t>Réception sujet Pré-TPI</t>
+  </si>
+  <si>
+    <t>Lecture, préparation questions pour Mr. Varela</t>
+  </si>
+  <si>
+    <t>Créations de VMs</t>
+  </si>
+  <si>
+    <t>Machines virtuelles VM1 et VM2 selon schéma. Pas touches aux réglages réseaux, NAT et DHCP reçu de l'école</t>
+  </si>
+  <si>
+    <t>Découverte cahier des charges</t>
+  </si>
+  <si>
+    <t>Réception Cahier des charges</t>
+  </si>
+  <si>
+    <t>Schéma logique</t>
+  </si>
+  <si>
+    <t>Préparation du schéma logique, avec les éléments actuels.</t>
+  </si>
+  <si>
+    <t>Création document principal</t>
+  </si>
+  <si>
+    <t>Mis en en place documentation</t>
   </si>
 </sst>
 </file>
@@ -482,7 +509,7 @@
   <dimension ref="A1:H270"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -490,7 +517,7 @@
     <col min="1" max="1" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="82.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="6.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="11.42578125" style="1"/>
@@ -556,7 +583,7 @@
       <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -583,7 +610,7 @@
       <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -610,7 +637,7 @@
       <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -631,52 +658,133 @@
       </c>
     </row>
     <row r="6" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="A6" s="8">
+        <v>44959</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.4375</v>
+      </c>
       <c r="H6" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.7777777777777735E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="A7" s="8">
+        <v>44959</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.4375</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0.4861111111111111</v>
+      </c>
       <c r="H7" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.8611111111111105E-2</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="A8" s="8">
+        <v>44959</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0.5</v>
+      </c>
       <c r="H8" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.3888888888888895E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="A9" s="8">
+        <v>44959</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="H9" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.041666666666663E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="F10" s="7"/>
+      <c r="A10" s="8">
+        <v>44959</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="F10" s="7">
+        <v>13.3</v>
+      </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-13.3</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
+      <c r="C11" s="9"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7">
@@ -686,6 +794,7 @@
     </row>
     <row r="12" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
+      <c r="C12" s="9"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7">
@@ -695,6 +804,7 @@
     </row>
     <row r="13" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
+      <c r="C13" s="9"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7">
@@ -704,6 +814,7 @@
     </row>
     <row r="14" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
+      <c r="C14" s="9"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7">
@@ -713,6 +824,7 @@
     </row>
     <row r="15" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
+      <c r="C15" s="9"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7">
@@ -722,6 +834,7 @@
     </row>
     <row r="16" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
+      <c r="C16" s="9"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7">
@@ -731,6 +844,7 @@
     </row>
     <row r="17" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
+      <c r="C17" s="9"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7">
@@ -740,6 +854,7 @@
     </row>
     <row r="18" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
+      <c r="C18" s="9"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7">
@@ -749,6 +864,7 @@
     </row>
     <row r="19" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
+      <c r="C19" s="9"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7">
@@ -758,6 +874,7 @@
     </row>
     <row r="20" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
+      <c r="C20" s="9"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7">
@@ -767,6 +884,7 @@
     </row>
     <row r="21" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
+      <c r="C21" s="9"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7">
@@ -776,6 +894,7 @@
     </row>
     <row r="22" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
+      <c r="C22" s="9"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7">
@@ -785,6 +904,7 @@
     </row>
     <row r="23" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
+      <c r="C23" s="9"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7">
@@ -794,6 +914,7 @@
     </row>
     <row r="24" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
+      <c r="C24" s="9"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7">
@@ -803,6 +924,7 @@
     </row>
     <row r="25" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
+      <c r="C25" s="9"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7">
@@ -812,6 +934,7 @@
     </row>
     <row r="26" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
+      <c r="C26" s="9"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7">
@@ -821,6 +944,7 @@
     </row>
     <row r="27" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
+      <c r="C27" s="9"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7">
@@ -830,6 +954,7 @@
     </row>
     <row r="28" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
+      <c r="C28" s="9"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7">
@@ -839,6 +964,7 @@
     </row>
     <row r="29" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
+      <c r="C29" s="9"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7">
@@ -848,6 +974,7 @@
     </row>
     <row r="30" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
+      <c r="C30" s="9"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7">
@@ -857,6 +984,7 @@
     </row>
     <row r="31" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
+      <c r="C31" s="9"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7">
@@ -866,6 +994,7 @@
     </row>
     <row r="32" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
+      <c r="C32" s="9"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7">
@@ -875,6 +1004,7 @@
     </row>
     <row r="33" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
+      <c r="C33" s="9"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7">
@@ -884,6 +1014,7 @@
     </row>
     <row r="34" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
+      <c r="C34" s="9"/>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
       <c r="H34" s="7">
@@ -893,6 +1024,7 @@
     </row>
     <row r="35" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
+      <c r="C35" s="9"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7">
@@ -902,6 +1034,7 @@
     </row>
     <row r="36" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
+      <c r="C36" s="9"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7">
@@ -910,6 +1043,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="C37" s="9"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7">
@@ -918,6 +1052,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="C38" s="9"/>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7">
@@ -926,6 +1061,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="C39" s="9"/>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7">
@@ -934,6 +1070,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="C40" s="9"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7">
@@ -942,6 +1079,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="C41" s="9"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7">
@@ -950,6 +1088,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="C42" s="9"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
       <c r="H42" s="7">
@@ -958,6 +1097,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="C43" s="9"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
       <c r="H43" s="7">
@@ -966,6 +1106,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="C44" s="9"/>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
       <c r="H44" s="7">
@@ -974,6 +1115,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="C45" s="9"/>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
       <c r="H45" s="7">
@@ -982,6 +1124,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="C46" s="9"/>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7">
@@ -990,6 +1133,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="C47" s="9"/>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
       <c r="H47" s="7">
@@ -998,6 +1142,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="C48" s="9"/>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
       <c r="H48" s="7">
@@ -1005,7 +1150,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="C49" s="9"/>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
       <c r="H49" s="7">
@@ -1013,7 +1159,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="C50" s="9"/>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
       <c r="H50" s="7">
@@ -1021,25 +1168,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="H51" s="7">
         <f>SUM(H2:H50)</f>
-        <v>0.23958333333333326</v>
-      </c>
-    </row>
-    <row r="52" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="6:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+        <v>-12.959722222222224</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="3:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="3:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="3:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="3:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="3:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="3:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="3:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="3:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="3:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="3:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="3:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="3:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
     <row r="65" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
     <row r="66" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
     <row r="67" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
@@ -1256,7 +1403,7 @@
           <x14:formula1>
             <xm:f>Paramètres!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C2</xm:sqref>
+          <xm:sqref>C2:C5 C7:C50</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1269,13 +1416,13 @@
   <dimension ref="A1:C288"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11.42578125" style="1"/>
   </cols>
@@ -1314,8 +1461,12 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="4">
+        <v>44959</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update diagrammes de Gantt
</commit_message>
<xml_diff>
--- a/Rendu/Journaux.xlsx
+++ b/Rendu/Journaux.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>Date</t>
   </si>
@@ -134,6 +134,24 @@
   </si>
   <si>
     <t>Mis en en place documentation</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Réception fortinet</t>
+  </si>
+  <si>
+    <t>Réception, déballage et inventaire du matériel reçu</t>
+  </si>
+  <si>
+    <t>Découverte du matériel</t>
+  </si>
+  <si>
+    <t>Lecture mode d'emploi et recherche documentation supplémentaire</t>
+  </si>
+  <si>
+    <t>Démarrage</t>
   </si>
 </sst>
 </file>
@@ -509,7 +527,7 @@
   <dimension ref="A1:H270"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -557,7 +575,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -584,7 +602,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>20</v>
@@ -611,7 +629,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>23</v>
@@ -638,7 +656,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>22</v>
@@ -665,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>30</v>
@@ -772,24 +790,51 @@
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="F10" s="7">
-        <v>13.3</v>
-      </c>
-      <c r="G10" s="7"/>
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="H10" s="7">
         <f t="shared" si="0"/>
-        <v>-13.3</v>
+        <v>1.3888888888888951E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="A11" s="8">
+        <v>44959</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="H11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.513888888888884E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -1171,7 +1216,7 @@
     <row r="51" spans="3:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="H51" s="7">
         <f>SUM(H2:H50)</f>
-        <v>-12.959722222222224</v>
+        <v>0.39930555555555541</v>
       </c>
     </row>
     <row r="52" spans="3:8" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25"/>
@@ -1401,9 +1446,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Paramètres!$A$2:$A$6</xm:f>
+            <xm:f>Paramètres!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C5 C7:C50</xm:sqref>
+          <xm:sqref>C2:C50</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1416,7 +1461,7 @@
   <dimension ref="A1:C288"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1467,7 +1512,9 @@
       <c r="B4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:3" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
@@ -2897,10 +2944,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2938,6 +2985,11 @@
         <v>18</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>